<commit_message>
added logout, multiple changes
</commit_message>
<xml_diff>
--- a/jobInfo.xlsx
+++ b/jobInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adriancondrea\Desktop\RPA\Hipo-UI-Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DD9E98-85E7-4566-929B-AB35FB22A6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179BE634-9D28-4DC1-9489-AFBDE334C3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="1920" windowWidth="16200" windowHeight="9398" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Cuvinte cheie</t>
   </si>
@@ -48,19 +48,16 @@
     <t>Oras</t>
   </si>
   <si>
-    <t>java developer</t>
-  </si>
-  <si>
     <t>IT-Software</t>
   </si>
   <si>
     <t>full-time</t>
   </si>
   <si>
-    <t>0 - 1 an experienta</t>
-  </si>
-  <si>
     <t>Cluj-Napoca</t>
+  </si>
+  <si>
+    <t>developer</t>
   </si>
 </sst>
 </file>
@@ -453,7 +450,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -484,19 +481,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>